<commit_message>
* Add COM support in python and plumbing to get Excel.Application object * Fix buffer overrun in object Cache * Ensure COM object is closed when XLL closes * Add settings option to change plugin auto load search pattern * Some docs/comments
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915F18F5-44F6-47C3-81CF-65D281AE39E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90173A93-D516-4928-97AF-3828310F7A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="192" windowWidth="14868" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>pySum</t>
   </si>
@@ -125,6 +124,9 @@
   </si>
   <si>
     <t>pyTestIter</t>
+  </si>
+  <si>
+    <t>pyTestCom()</t>
   </si>
 </sst>
 </file>
@@ -586,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,16 +621,16 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="e">
-        <f ca="1">C2=D2</f>
-        <v>#VALUE!</v>
+      <c r="B2" t="b">
+        <f>C2=D2</f>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2" t="e">
-        <f ca="1">_xll.pySum(1,2,3)</f>
-        <v>#VALUE!</v>
+      <c r="D2">
+        <f>_xll.pySum(1,2,3)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -636,15 +638,15 @@
         <v>5</v>
       </c>
       <c r="B3" t="b">
-        <f ca="1">NOT(ISERROR(FIND("Error",D3)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(FIND("Error",D3)))</f>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="e">
-        <f ca="1">_xll.pySum(1,2)</f>
-        <v>#VALUE!</v>
+      <c r="D3" t="str">
+        <f>_xll.pySum(1,2)</f>
+        <v>Error reading 'z' arg #3: Missing argument</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -654,16 +656,16 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="e">
-        <f ca="1">C5=D5</f>
-        <v>#VALUE!</v>
+      <c r="B5" t="b">
+        <f>C5=D5</f>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>9</v>
       </c>
-      <c r="D5" t="e">
-        <f ca="1">_xll.pySumNums(1,2,3)</f>
-        <v>#VALUE!</v>
+      <c r="D5">
+        <f>_xll.pySumNums(1,2,3)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -671,77 +673,77 @@
         <v>4</v>
       </c>
       <c r="B6" t="b">
-        <f ca="1">NOT(ISERROR(FIND("Error",C6)))</f>
-        <v>0</v>
-      </c>
-      <c r="C6" t="e">
-        <f ca="1">_xll.pySumNums(1,2,3.2)</f>
-        <v>#VALUE!</v>
+        <f>NOT(ISERROR(FIND("Error",C6)))</f>
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xll.pySumNums(1,2,3.2)</f>
+        <v xml:space="preserve">Error reading 'a' arg #3: Failed converting 3.200000: </v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="e">
-        <f ca="1">D8=C8</f>
-        <v>#VALUE!</v>
+      <c r="B8" t="b">
+        <f>D8=C8</f>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" t="e">
-        <f ca="1">_xll.pyRoundTrip(C8)</f>
-        <v>#VALUE!</v>
+      <c r="D8">
+        <f>_xll.pyRoundTrip(C8)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="e">
-        <f ca="1">D9=C9</f>
-        <v>#VALUE!</v>
+      <c r="B9" t="b">
+        <f>D9=C9</f>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>3.3</v>
       </c>
-      <c r="D9" t="e">
-        <f ca="1">_xll.pyRoundTrip(C9)</f>
-        <v>#VALUE!</v>
+      <c r="D9">
+        <f>_xll.pyRoundTrip(C9)</f>
+        <v>3.3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="e">
-        <f ca="1">D10=C10</f>
-        <v>#VALUE!</v>
+      <c r="B10" t="b">
+        <f>D10=C10</f>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>42736</v>
       </c>
-      <c r="D10" s="3" t="e">
-        <f ca="1">_xll.pyRoundTrip(C10)</f>
-        <v>#VALUE!</v>
+      <c r="D10" s="3">
+        <f>_xll.pyRoundTrip(C10)</f>
+        <v>42736</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="e">
-        <f ca="1">C11=D11</f>
-        <v>#VALUE!</v>
+      <c r="B11" t="b">
+        <f>C11=D11</f>
+        <v>1</v>
       </c>
       <c r="C11">
         <f>SUM(E11:G11)</f>
         <v>6</v>
       </c>
-      <c r="D11" t="e">
-        <f t="array" aca="1" ref="D11" ca="1">SUM(_xll.pyRoundTrip(E11:G11))</f>
-        <v>#VALUE!</v>
+      <c r="D11">
+        <f t="array" ref="D11">SUM(_xll.pyRoundTrip(E11:G11))</f>
+        <v>6</v>
       </c>
       <c r="E11" s="9">
         <v>1</v>
@@ -758,50 +760,50 @@
         <v>10</v>
       </c>
       <c r="B12" t="b">
-        <f ca="1">ISNA(D12)</f>
-        <v>0</v>
+        <f>ISNA(D12)</f>
+        <v>1</v>
       </c>
       <c r="C12" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D12" t="e">
-        <f ca="1">(_xll.pyRoundTrip(E12:G12))</f>
-        <v>#VALUE!</v>
+        <f>(_xll.pyRoundTrip(E12:G12))</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="e">
-        <f ca="1">C13=D13</f>
-        <v>#VALUE!</v>
+      <c r="B13" t="b">
+        <f>C13=D13</f>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>C11</f>
         <v>6</v>
       </c>
-      <c r="D13" t="e">
-        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
-        <v>#VALUE!</v>
+      <c r="D13">
+        <f>SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="e">
-        <f ca="1">C15=D15</f>
-        <v>#VALUE!</v>
+      <c r="B15" t="b">
+        <f>C15=D15</f>
+        <v>1</v>
       </c>
       <c r="C15">
         <f t="array" ref="C15">SUM(F15:H15*E15)</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="D15" t="e">
-        <f ca="1">SUM(_xll.pyTestArr1d(F15:H15,E15))</f>
-        <v>#VALUE!</v>
+      <c r="D15">
+        <f>SUM(_xll.pyTestArr1d(F15:H15,E15))</f>
+        <v>18.600000000000001</v>
       </c>
       <c r="E15">
         <v>3.1</v>
@@ -821,15 +823,15 @@
         <v>12</v>
       </c>
       <c r="B16" t="b">
-        <f ca="1">NOT(ISERROR(FIND("Error",D16)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(FIND("Error",D16)))</f>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="e">
-        <f ca="1">_xll.pyTestArr1d(F16:H17,E16)</f>
-        <v>#VALUE!</v>
+      <c r="D16" t="str">
+        <f>_xll.pyTestArr1d(F16:H17,E16)</f>
+        <v>Error reading 'x' arg #1: Expecting a 1-dim array</v>
       </c>
       <c r="E16">
         <v>3.1</v>
@@ -843,9 +845,9 @@
       <c r="H16" s="6">
         <v>3</v>
       </c>
-      <c r="K16" t="e">
-        <f ca="1">D16</f>
-        <v>#VALUE!</v>
+      <c r="K16" t="str">
+        <f>D16</f>
+        <v>Error reading 'x' arg #1: Expecting a 1-dim array</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -863,17 +865,17 @@
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="e">
-        <f ca="1">C19=D19</f>
-        <v>#VALUE!</v>
+      <c r="B19" t="b">
+        <f>C19=D19</f>
+        <v>1</v>
       </c>
       <c r="C19">
         <f>SUM(E19:F20)</f>
         <v>10</v>
       </c>
-      <c r="D19" t="e">
-        <f ca="1">SUM(_xll.pyTestArr2d(E19:F20))</f>
-        <v>#VALUE!</v>
+      <c r="D19">
+        <f>SUM(_xll.pyTestArr2d(E19:F20))</f>
+        <v>10</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -886,17 +888,17 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="e">
-        <f ca="1">C20=D20</f>
-        <v>#VALUE!</v>
+      <c r="B20" t="b">
+        <f>C20=D20</f>
+        <v>1</v>
       </c>
       <c r="C20">
         <f>C19</f>
         <v>10</v>
       </c>
-      <c r="D20" t="e">
-        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
-        <v>#VALUE!</v>
+      <c r="D20">
+        <f>SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
+        <v>10</v>
       </c>
       <c r="E20" s="7">
         <v>3</v>
@@ -909,17 +911,17 @@
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="e">
-        <f ca="1">C23=D23</f>
-        <v>#VALUE!</v>
+      <c r="B23" t="b">
+        <f>C23=D23</f>
+        <v>1</v>
       </c>
       <c r="C23" t="str">
         <f>F24</f>
         <v>parrot</v>
       </c>
-      <c r="D23" t="e">
-        <f ca="1">_xll.pyTestKwargs(E24,E23:F24)</f>
-        <v>#VALUE!</v>
+      <c r="D23" t="str">
+        <f>_xll.pyTestKwargs(E24,E23:F24)</f>
+        <v>parrot</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -932,17 +934,17 @@
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="e">
-        <f ca="1">C24=D24</f>
-        <v>#VALUE!</v>
+      <c r="B24" t="b">
+        <f>C24=D24</f>
+        <v>1</v>
       </c>
       <c r="C24" t="str">
         <f>C23</f>
         <v>parrot</v>
       </c>
-      <c r="D24" t="e">
-        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
-        <v>#VALUE!</v>
+      <c r="D24" t="str">
+        <f>_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
+        <v>parrot</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>19</v>
@@ -955,70 +957,79 @@
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="e">
-        <f ca="1">C27=D27</f>
-        <v>#VALUE!</v>
+      <c r="B27" t="b">
+        <f>C27=D27</f>
+        <v>1</v>
       </c>
       <c r="C27" t="str">
         <f>E27</f>
         <v>foo</v>
       </c>
-      <c r="D27" s="4" t="e">
-        <f ca="1">_xll.pyTestAsync(E27,1)</f>
-        <v>#VALUE!</v>
+      <c r="D27" s="4" t="str">
+        <f>_xll.pyTestAsync(E27,1)</f>
+        <v>foo</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" t="e">
-        <f ca="1">C28=D28</f>
-        <v>#VALUE!</v>
+      <c r="B28" t="b">
+        <f>C28=D28</f>
+        <v>1</v>
       </c>
       <c r="C28" t="str">
         <f>C27</f>
         <v>foo</v>
       </c>
-      <c r="D28" t="e">
-        <f ca="1">_xll.pyTestAsyncThread(E27,1)</f>
-        <v>#VALUE!</v>
+      <c r="D28" t="str">
+        <f>_xll.pyTestAsyncThread(E27,1)</f>
+        <v>foo</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="e">
-        <f ca="1">C30=D30</f>
-        <v>#VALUE!</v>
+      <c r="B30" t="b">
+        <f>C30=D30</f>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D30" t="e">
-        <f ca="1">_xll.pyTestCache(E30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E30" t="e">
-        <f ca="1">_xll.pyTestCache()</f>
-        <v>#VALUE!</v>
+      <c r="D30" t="str">
+        <f>_xll.pyTestCache(E30)</f>
+        <v>Hello world</v>
+      </c>
+      <c r="E30" t="str">
+        <f>_xll.pyTestCache()</f>
+        <v>欣[PythonTest.xlsx]Sheet1!R30C5_x0000__x0000__x0000__x0000_</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="e">
-        <f ca="1">C32=D32</f>
-        <v>#VALUE!</v>
+      <c r="B32" t="b">
+        <f>C32=D32</f>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="D32" t="e">
-        <f ca="1">SUM(_xll.pyTestIter(4,1))</f>
-        <v>#VALUE!</v>
+      <c r="D32">
+        <f>SUM(_xll.pyTestIter(4,1))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="str">
+        <f>_xll.pyTestCom()</f>
+        <v>{90160000-000F-0000-1000-0000000FF1CE}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Add support for passing range referencs to UDFs * Add a fair bit of documentation * Allow fetching from registry in settings file, use this to simplify python loading
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90173A93-D516-4928-97AF-3828310F7A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FB92C3-605A-4C1A-BD99-9E9770597487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="192" windowWidth="14868" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2472" yWindow="1356" windowWidth="14868" windowHeight="11604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>pySum</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>pyTestCom()</t>
+  </si>
+  <si>
+    <t>pyTestRange()</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,7 +603,7 @@
     <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -617,133 +620,133 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="b">
-        <f>C2=D2</f>
-        <v>1</v>
+      <c r="B2" t="e">
+        <f ca="1">C2=D2</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2">
-        <f>_xll.pySum(1,2,3)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D2" t="e">
+        <f ca="1">_xll.pySum(1,2,3)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="b">
-        <f>NOT(ISERROR(FIND("Error",D3)))</f>
-        <v>1</v>
+        <f ca="1">NOT(ISERROR(FIND("Error",D3)))</f>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="str">
-        <f>_xll.pySum(1,2)</f>
-        <v>Error reading 'z' arg #3: Missing argument</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D3" t="e">
+        <f ca="1">_xll.pySum(1,2)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="b">
-        <f>C5=D5</f>
-        <v>1</v>
+      <c r="B5" t="e">
+        <f ca="1">C5=D5</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C5">
         <v>9</v>
       </c>
-      <c r="D5">
-        <f>_xll.pySumNums(1,2,3)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D5" t="e">
+        <f ca="1">_xll.pySumNums(1,2,3)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="b">
-        <f>NOT(ISERROR(FIND("Error",C6)))</f>
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <f>_xll.pySumNums(1,2,3.2)</f>
-        <v xml:space="preserve">Error reading 'a' arg #3: Failed converting 3.200000: </v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <f ca="1">NOT(ISERROR(FIND("Error",C6)))</f>
+        <v>0</v>
+      </c>
+      <c r="C6" t="e">
+        <f ca="1">_xll.pySumNums(1,2,3.2)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="b">
-        <f>D8=C8</f>
-        <v>1</v>
+      <c r="B8" t="e">
+        <f ca="1">D8=C8</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8">
-        <f>_xll.pyRoundTrip(C8)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8" t="e">
+        <f ca="1">_xll.pyRoundTrip(C8)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="b">
-        <f>D9=C9</f>
-        <v>1</v>
+      <c r="B9" t="e">
+        <f ca="1">D9=C9</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C9">
         <v>3.3</v>
       </c>
-      <c r="D9">
-        <f>_xll.pyRoundTrip(C9)</f>
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" t="e">
+        <f ca="1">_xll.pyRoundTrip(C9)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="b">
-        <f>D10=C10</f>
-        <v>1</v>
+      <c r="B10" t="e">
+        <f ca="1">D10=C10</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C10" s="3">
         <v>42736</v>
       </c>
-      <c r="D10" s="3">
-        <f>_xll.pyRoundTrip(C10)</f>
-        <v>42736</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="3" t="e">
+        <f ca="1">_xll.pyRoundTrip(C10)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="b">
-        <f>C11=D11</f>
-        <v>1</v>
+      <c r="B11" t="e">
+        <f ca="1">C11=D11</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C11">
         <f>SUM(E11:G11)</f>
         <v>6</v>
       </c>
-      <c r="D11">
-        <f t="array" ref="D11">SUM(_xll.pyRoundTrip(E11:G11))</f>
-        <v>6</v>
+      <c r="D11" t="e">
+        <f t="array" aca="1" ref="D11" ca="1">SUM(_xll.pyRoundTrip(E11:G11))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E11" s="9">
         <v>1</v>
@@ -755,55 +758,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="b">
-        <f>ISNA(D12)</f>
-        <v>1</v>
+        <f ca="1">ISNA(D12)</f>
+        <v>0</v>
       </c>
       <c r="C12" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D12" t="e">
-        <f>(_xll.pyRoundTrip(E12:G12))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <f ca="1">(_xll.pyRoundTrip(E12:G12))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="b">
-        <f>C13=D13</f>
-        <v>1</v>
+      <c r="B13" t="e">
+        <f ca="1">C13=D13</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C13">
         <f>C11</f>
         <v>6</v>
       </c>
-      <c r="D13">
-        <f>SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D13" t="e">
+        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="b">
-        <f>C15=D15</f>
-        <v>1</v>
+      <c r="B15" t="e">
+        <f ca="1">C15=D15</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C15">
         <f t="array" ref="C15">SUM(F15:H15*E15)</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="D15">
-        <f>SUM(_xll.pyTestArr1d(F15:H15,E15))</f>
-        <v>18.600000000000001</v>
+      <c r="D15" t="e">
+        <f ca="1">SUM(_xll.pyTestArr1d(F15:H15,E15))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E15">
         <v>3.1</v>
@@ -818,20 +821,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="b">
-        <f>NOT(ISERROR(FIND("Error",D16)))</f>
-        <v>1</v>
+        <f ca="1">NOT(ISERROR(FIND("Error",D16)))</f>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="str">
-        <f>_xll.pyTestArr1d(F16:H17,E16)</f>
-        <v>Error reading 'x' arg #1: Expecting a 1-dim array</v>
+      <c r="D16" t="e">
+        <f ca="1">_xll.pyTestArr1d(F16:H17,E16)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E16">
         <v>3.1</v>
@@ -844,10 +847,6 @@
       </c>
       <c r="H16" s="6">
         <v>3</v>
-      </c>
-      <c r="K16" t="str">
-        <f>D16</f>
-        <v>Error reading 'x' arg #1: Expecting a 1-dim array</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -865,17 +864,17 @@
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="b">
-        <f>C19=D19</f>
-        <v>1</v>
+      <c r="B19" t="e">
+        <f ca="1">C19=D19</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C19">
         <f>SUM(E19:F20)</f>
         <v>10</v>
       </c>
-      <c r="D19">
-        <f>SUM(_xll.pyTestArr2d(E19:F20))</f>
-        <v>10</v>
+      <c r="D19" t="e">
+        <f ca="1">SUM(_xll.pyTestArr2d(E19:F20))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -888,17 +887,17 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="b">
-        <f>C20=D20</f>
-        <v>1</v>
+      <c r="B20" t="e">
+        <f ca="1">C20=D20</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C20">
         <f>C19</f>
         <v>10</v>
       </c>
-      <c r="D20">
-        <f>SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
-        <v>10</v>
+      <c r="D20" t="e">
+        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E20" s="7">
         <v>3</v>
@@ -911,17 +910,17 @@
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="b">
-        <f>C23=D23</f>
-        <v>1</v>
+      <c r="B23" t="e">
+        <f ca="1">C23=D23</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C23" t="str">
         <f>F24</f>
         <v>parrot</v>
       </c>
-      <c r="D23" t="str">
-        <f>_xll.pyTestKwargs(E24,E23:F24)</f>
-        <v>parrot</v>
+      <c r="D23" t="e">
+        <f ca="1">_xll.pyTestKwargs(E24,E23:F24)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -934,17 +933,17 @@
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="b">
-        <f>C24=D24</f>
-        <v>1</v>
+      <c r="B24" t="e">
+        <f ca="1">C24=D24</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C24" t="str">
         <f>C23</f>
         <v>parrot</v>
       </c>
-      <c r="D24" t="str">
-        <f>_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
-        <v>parrot</v>
+      <c r="D24" t="e">
+        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>19</v>
@@ -957,79 +956,110 @@
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="b">
-        <f>C27=D27</f>
-        <v>1</v>
+      <c r="B27" t="e">
+        <f ca="1">C27=D27</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C27" t="str">
         <f>E27</f>
         <v>foo</v>
       </c>
-      <c r="D27" s="4" t="str">
-        <f>_xll.pyTestAsync(E27,1)</f>
-        <v>foo</v>
+      <c r="D27" s="4" t="e">
+        <f ca="1">_xll.pyTestAsync(E27,1)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" t="b">
-        <f>C28=D28</f>
-        <v>1</v>
+      <c r="B28" t="e">
+        <f ca="1">C28=D28</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C28" t="str">
         <f>C27</f>
         <v>foo</v>
       </c>
-      <c r="D28" t="str">
-        <f>_xll.pyTestAsyncThread(E27,1)</f>
-        <v>foo</v>
+      <c r="D28" t="e">
+        <f ca="1">_xll.pyTestAsyncThread(E27,1)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="b">
-        <f>C30=D30</f>
-        <v>1</v>
+      <c r="B30" t="e">
+        <f ca="1">C30=D30</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D30" t="str">
-        <f>_xll.pyTestCache(E30)</f>
-        <v>Hello world</v>
-      </c>
-      <c r="E30" t="str">
-        <f>_xll.pyTestCache()</f>
-        <v>欣[PythonTest.xlsx]Sheet1!R30C5_x0000__x0000__x0000__x0000_</v>
+      <c r="D30" t="e">
+        <f ca="1">_xll.pyTestCache(E30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E30" t="e">
+        <f ca="1">_xll.pyTestCache()</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="b">
-        <f>C32=D32</f>
-        <v>1</v>
+      <c r="B32" t="e">
+        <f ca="1">C32=D32</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="D32">
-        <f>SUM(_xll.pyTestIter(4,1))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32" t="e">
+        <f ca="1">SUM(_xll.pyTestIter(4,1))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="str">
-        <f>_xll.pyTestCom()</f>
-        <v>{90160000-000F-0000-1000-0000000FF1CE}</v>
+      <c r="B34" t="e">
+        <f ca="1">_xll.pyTestCom()</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="e">
+        <f ca="1">C36=D36</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C36" t="str">
+        <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename")),100)&amp;"!"&amp;ADDRESS(ROW(F37),COLUMN(F37),4)</f>
+        <v>[PythonTest.xlsx]Sheet1!F37</v>
+      </c>
+      <c r="D36" t="e">
+        <f t="array" aca="1" ref="D36" ca="1">_xll.pyTestRange(E36:F37)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Reorg so that plugins are in separate solutions.  Things were getting messy with different python versions * Change ini file loading so that each plugin has it's own ini.  Gives better separation than all piling into the main one * Allow object cache concurrency
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FB92C3-605A-4C1A-BD99-9E9770597487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9BE84-C9AE-4989-90F9-8B89BCF4CE9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2472" yWindow="1356" windowWidth="14868" windowHeight="11604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,7 +594,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,6 +715,10 @@
         <f ca="1">_xll.pyRoundTrip(C9)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H9" t="e">
+        <f>xlo</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -788,7 +792,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="e">
-        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
+        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloPush(E11:G11)))</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -896,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="e">
-        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
+        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloPush(E19:F20)))</f>
         <v>#VALUE!</v>
       </c>
       <c r="E20" s="7">
@@ -942,7 +946,7 @@
         <v>parrot</v>
       </c>
       <c r="D24" t="e">
-        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
+        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloPush(E23:F24))</f>
         <v>#VALUE!</v>
       </c>
       <c r="E24" s="7" t="s">

</xml_diff>

<commit_message>
Fix vcproj file paths and test spreadsheet
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9BE84-C9AE-4989-90F9-8B89BCF4CE9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3478C961-F4A1-4589-89DE-CACA6D0A5C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2472" yWindow="1356" windowWidth="14868" windowHeight="11604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>pySum</t>
   </si>
@@ -130,6 +131,18 @@
   </si>
   <si>
     <t>pyTestRange()</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -593,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,7 +805,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="e">
-        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloPush(E11:G11)))</f>
+        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -900,7 +913,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="e">
-        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloPush(E19:F20)))</f>
+        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
         <v>#VALUE!</v>
       </c>
       <c r="E20" s="7">
@@ -946,7 +959,7 @@
         <v>parrot</v>
       </c>
       <c r="D24" t="e">
-        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloPush(E23:F24))</f>
+        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
         <v>#VALUE!</v>
       </c>
       <c r="E24" s="7" t="s">
@@ -1045,7 +1058,7 @@
       </c>
       <c r="C36" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename")),100)&amp;"!"&amp;ADDRESS(ROW(F37),COLUMN(F37),4)</f>
-        <v>[PythonTest.xlsx]Sheet1!F37</v>
+        <v>[PythonTest.xlsx]Sheet2!F37</v>
       </c>
       <c r="D36" t="e">
         <f t="array" aca="1" ref="D36" ca="1">_xll.pyTestRange(E36:F37)</f>
@@ -1070,4 +1083,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECBB5EF-8BCA-472B-B4EA-42C7538449FE}">
+  <dimension ref="B2:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="e">
+        <f ca="1">_xll.xloRef(D2:E3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="e">
+        <f ca="1">_xll.xloRef(D5:E6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" t="e">
+        <f t="array" aca="1" ref="D5:E6" ca="1">_xll.xloObj(B2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E6" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D8" t="e">
+        <f t="array" aca="1" ref="D8:E9" ca="1">_xll.xloObj($B$2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E8" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E9" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D11" t="e">
+        <f t="array" aca="1" ref="D11:E12" ca="1">_xll.xloObj($B$2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E11" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D12" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D14" t="e">
+        <f t="array" aca="1" ref="D14:E15" ca="1">_xll.xloObj($B$5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D15" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E15" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update python docs and add release script
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3478C961-F4A1-4589-89DE-CACA6D0A5C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BD8955-D969-452A-9336-986807517A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7668" yWindow="1476" windowWidth="14868" windowHeight="11604" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,16 +637,16 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="e">
-        <f ca="1">C2=D2</f>
-        <v>#VALUE!</v>
+      <c r="B2" t="b">
+        <f>C2=D2</f>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2" t="e">
-        <f ca="1">_xll.pySum(1,2,3)</f>
-        <v>#VALUE!</v>
+      <c r="D2">
+        <f>_xll.pySum(1,2,3)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -654,15 +654,15 @@
         <v>5</v>
       </c>
       <c r="B3" t="b">
-        <f ca="1">NOT(ISERROR(FIND("Error",D3)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(FIND("Error",D3)))</f>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="e">
-        <f ca="1">_xll.pySum(1,2)</f>
-        <v>#VALUE!</v>
+      <c r="D3" t="str">
+        <f>_xll.pySum(1,2)</f>
+        <v>Error reading 'z' arg #3: Missing argument</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -672,16 +672,16 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="e">
-        <f ca="1">C5=D5</f>
-        <v>#VALUE!</v>
+      <c r="B5" t="b">
+        <f>C5=D5</f>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>9</v>
       </c>
-      <c r="D5" t="e">
-        <f ca="1">_xll.pySumNums(1,2,3)</f>
-        <v>#VALUE!</v>
+      <c r="D5">
+        <f>_xll.pySumNums(1,2,3)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -689,44 +689,44 @@
         <v>4</v>
       </c>
       <c r="B6" t="b">
-        <f ca="1">NOT(ISERROR(FIND("Error",C6)))</f>
-        <v>0</v>
-      </c>
-      <c r="C6" t="e">
-        <f ca="1">_xll.pySumNums(1,2,3.2)</f>
-        <v>#VALUE!</v>
+        <f>NOT(ISERROR(FIND("Error",C6)))</f>
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xll.pySumNums(1,2,3.2)</f>
+        <v xml:space="preserve">Error reading 'a' arg #3: Failed converting 3.200000: </v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="e">
-        <f ca="1">D8=C8</f>
-        <v>#VALUE!</v>
+      <c r="B8" t="b">
+        <f>D8=C8</f>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" t="e">
-        <f ca="1">_xll.pyRoundTrip(C8)</f>
-        <v>#VALUE!</v>
+      <c r="D8">
+        <f>_xll.pyRoundTrip(C8)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="e">
-        <f ca="1">D9=C9</f>
-        <v>#VALUE!</v>
+      <c r="B9" t="b">
+        <f>D9=C9</f>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>3.3</v>
       </c>
-      <c r="D9" t="e">
-        <f ca="1">_xll.pyRoundTrip(C9)</f>
-        <v>#VALUE!</v>
+      <c r="D9">
+        <f>_xll.pyRoundTrip(C9)</f>
+        <v>3.3</v>
       </c>
       <c r="H9" t="e">
         <f>xlo</f>
@@ -737,33 +737,33 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="e">
-        <f ca="1">D10=C10</f>
-        <v>#VALUE!</v>
+      <c r="B10" t="b">
+        <f>D10=C10</f>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>42736</v>
       </c>
-      <c r="D10" s="3" t="e">
-        <f ca="1">_xll.pyRoundTrip(C10)</f>
-        <v>#VALUE!</v>
+      <c r="D10" s="3">
+        <f>_xll.pyRoundTrip(C10)</f>
+        <v>42736</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="e">
-        <f ca="1">C11=D11</f>
-        <v>#VALUE!</v>
+      <c r="B11" t="b">
+        <f>C11=D11</f>
+        <v>1</v>
       </c>
       <c r="C11">
         <f>SUM(E11:G11)</f>
         <v>6</v>
       </c>
-      <c r="D11" t="e">
-        <f t="array" aca="1" ref="D11" ca="1">SUM(_xll.pyRoundTrip(E11:G11))</f>
-        <v>#VALUE!</v>
+      <c r="D11">
+        <f t="array" ref="D11">SUM(_xll.pyRoundTrip(E11:G11))</f>
+        <v>6</v>
       </c>
       <c r="E11" s="9">
         <v>1</v>
@@ -780,50 +780,50 @@
         <v>10</v>
       </c>
       <c r="B12" t="b">
-        <f ca="1">ISNA(D12)</f>
-        <v>0</v>
+        <f>ISNA(D12)</f>
+        <v>1</v>
       </c>
       <c r="C12" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="D12" t="e">
-        <f ca="1">(_xll.pyRoundTrip(E12:G12))</f>
-        <v>#VALUE!</v>
+        <f>(_xll.pyRoundTrip(E12:G12))</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="e">
-        <f ca="1">C13=D13</f>
-        <v>#VALUE!</v>
+      <c r="B13" t="b">
+        <f>C13=D13</f>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>C11</f>
         <v>6</v>
       </c>
-      <c r="D13" t="e">
-        <f ca="1">SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
-        <v>#VALUE!</v>
+      <c r="D13">
+        <f>SUM(_xll.pyRoundTrip(_xll.xloRef(E11:G11)))</f>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="e">
-        <f ca="1">C15=D15</f>
-        <v>#VALUE!</v>
+      <c r="B15" t="b">
+        <f>C15=D15</f>
+        <v>1</v>
       </c>
       <c r="C15">
         <f t="array" ref="C15">SUM(F15:H15*E15)</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="D15" t="e">
-        <f ca="1">SUM(_xll.pyTestArr1d(F15:H15,E15))</f>
-        <v>#VALUE!</v>
+      <c r="D15">
+        <f>SUM(_xll.pyTestArr1d(F15:H15,E15))</f>
+        <v>18.600000000000001</v>
       </c>
       <c r="E15">
         <v>3.1</v>
@@ -843,15 +843,15 @@
         <v>12</v>
       </c>
       <c r="B16" t="b">
-        <f ca="1">NOT(ISERROR(FIND("Error",D16)))</f>
-        <v>0</v>
+        <f>NOT(ISERROR(FIND("Error",D16)))</f>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="e">
-        <f ca="1">_xll.pyTestArr1d(F16:H17,E16)</f>
-        <v>#VALUE!</v>
+      <c r="D16" t="str">
+        <f>_xll.pyTestArr1d(F16:H17,E16)</f>
+        <v>Error reading 'x' arg #1: Expecting a 1-dim array</v>
       </c>
       <c r="E16">
         <v>3.1</v>
@@ -881,17 +881,17 @@
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="e">
-        <f ca="1">C19=D19</f>
-        <v>#VALUE!</v>
+      <c r="B19" t="b">
+        <f>C19=D19</f>
+        <v>1</v>
       </c>
       <c r="C19">
         <f>SUM(E19:F20)</f>
         <v>10</v>
       </c>
-      <c r="D19" t="e">
-        <f ca="1">SUM(_xll.pyTestArr2d(E19:F20))</f>
-        <v>#VALUE!</v>
+      <c r="D19">
+        <f>SUM(_xll.pyTestArr2d(E19:F20))</f>
+        <v>10</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -904,17 +904,17 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="e">
-        <f ca="1">C20=D20</f>
-        <v>#VALUE!</v>
+      <c r="B20" t="b">
+        <f>C20=D20</f>
+        <v>1</v>
       </c>
       <c r="C20">
         <f>C19</f>
         <v>10</v>
       </c>
-      <c r="D20" t="e">
-        <f ca="1">SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
-        <v>#VALUE!</v>
+      <c r="D20">
+        <f>SUM(_xll.pyTestArr2d(_xll.xloRef(E19:F20)))</f>
+        <v>10</v>
       </c>
       <c r="E20" s="7">
         <v>3</v>
@@ -927,17 +927,17 @@
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="e">
-        <f ca="1">C23=D23</f>
-        <v>#VALUE!</v>
+      <c r="B23" t="b">
+        <f>C23=D23</f>
+        <v>1</v>
       </c>
       <c r="C23" t="str">
         <f>F24</f>
         <v>parrot</v>
       </c>
-      <c r="D23" t="e">
-        <f ca="1">_xll.pyTestKwargs(E24,E23:F24)</f>
-        <v>#VALUE!</v>
+      <c r="D23" t="str">
+        <f>_xll.pyTestKwargs(E24,E23:F24)</f>
+        <v>parrot</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -950,17 +950,17 @@
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="e">
-        <f ca="1">C24=D24</f>
-        <v>#VALUE!</v>
+      <c r="B24" t="b">
+        <f>C24=D24</f>
+        <v>1</v>
       </c>
       <c r="C24" t="str">
         <f>C23</f>
         <v>parrot</v>
       </c>
-      <c r="D24" t="e">
-        <f ca="1">_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
-        <v>#VALUE!</v>
+      <c r="D24" t="str">
+        <f>_xll.pyTestKwargs(E24,_xll.xloRef(E23:F24))</f>
+        <v>parrot</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>19</v>
@@ -973,96 +973,96 @@
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="e">
-        <f ca="1">C27=D27</f>
-        <v>#VALUE!</v>
+      <c r="B27" t="b">
+        <f>C27=D27</f>
+        <v>1</v>
       </c>
       <c r="C27" t="str">
         <f>E27</f>
         <v>foo</v>
       </c>
-      <c r="D27" s="4" t="e">
-        <f ca="1">_xll.pyTestAsync(E27,1)</f>
-        <v>#VALUE!</v>
+      <c r="D27" s="4" t="str">
+        <f>_xll.pyTestAsync(E27,1)</f>
+        <v>foo</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" t="e">
-        <f ca="1">C28=D28</f>
-        <v>#VALUE!</v>
+      <c r="B28" t="b">
+        <f>C28=D28</f>
+        <v>1</v>
       </c>
       <c r="C28" t="str">
         <f>C27</f>
         <v>foo</v>
       </c>
-      <c r="D28" t="e">
-        <f ca="1">_xll.pyTestAsyncThread(E27,1)</f>
-        <v>#VALUE!</v>
+      <c r="D28" t="str">
+        <f>_xll.pyTestAsyncThread(E27,1)</f>
+        <v>foo</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="e">
-        <f ca="1">C30=D30</f>
-        <v>#VALUE!</v>
+      <c r="B30" t="b">
+        <f>C30=D30</f>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D30" t="e">
-        <f ca="1">_xll.pyTestCache(E30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E30" t="e">
-        <f ca="1">_xll.pyTestCache()</f>
-        <v>#VALUE!</v>
+      <c r="D30" t="str">
+        <f>_xll.pyTestCache(E30)</f>
+        <v>Hello world</v>
+      </c>
+      <c r="E30" t="str">
+        <f>_xll.pyTestCache()</f>
+        <v>欣[PythonTest.xlsx]Sheet1!R30C5_x0000__x0000__x0000__x0000_</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="e">
-        <f ca="1">C32=D32</f>
-        <v>#VALUE!</v>
+      <c r="B32" t="b">
+        <f>C32=D32</f>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="D32" t="e">
-        <f ca="1">SUM(_xll.pyTestIter(4,1))</f>
-        <v>#VALUE!</v>
+      <c r="D32">
+        <f>SUM(_xll.pyTestIter(4,1))</f>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="e">
-        <f ca="1">_xll.pyTestCom()</f>
-        <v>#VALUE!</v>
+      <c r="B34" t="str">
+        <f>_xll.pyTestCom()</f>
+        <v>{90160000-000F-0000-1000-0000000FF1CE}</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36" t="e">
+      <c r="B36" t="b">
         <f ca="1">C36=D36</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="C36" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename")),100)&amp;"!"&amp;ADDRESS(ROW(F37),COLUMN(F37),4)</f>
         <v>[PythonTest.xlsx]Sheet2!F37</v>
       </c>
-      <c r="D36" t="e">
+      <c r="D36" t="str">
         <f t="array" aca="1" ref="D36" ca="1">_xll.pyTestRange(E36:F37)</f>
-        <v>#VALUE!</v>
+        <v>[PythonTest.xlsx]Sheet2!F37</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1090,15 +1090,15 @@
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" t="e">
-        <f ca="1">_xll.xloRef(D2:E3)</f>
-        <v>#VALUE!</v>
+      <c r="B2" t="str">
+        <f>_xll.xloRef(D2:E3)</f>
+        <v>永[PythonTest.xlsx]Sheet2!R2C2_x0000__x0000__x0000__x0000_</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
@@ -1116,87 +1116,75 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="e">
-        <f ca="1">_xll.xloRef(D5:E6)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D5" t="e">
-        <f t="array" aca="1" ref="D5:E6" ca="1">_xll.xloObj(B2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B5" t="str">
+        <f>_xll.xloRef(D5:E6)</f>
+        <v>永[PythonTest.xlsx]Sheet2!R5C2_x0000__x0000__x0000__x0000_</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="array" ref="D5:E6">_xll.xloVal(B2)</f>
+        <v>X</v>
+      </c>
+      <c r="E5" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D6" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E6" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D6" t="str">
+        <v>C</v>
+      </c>
+      <c r="E6" t="str">
+        <v>D</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D8" t="e">
-        <f t="array" aca="1" ref="D8:E9" ca="1">_xll.xloObj($B$2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E8" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D8" t="str">
+        <f t="array" ref="D8:E9">_xll.xloVal($B$2)</f>
+        <v>X</v>
+      </c>
+      <c r="E8" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E9" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D9" t="str">
+        <v>C</v>
+      </c>
+      <c r="E9" t="str">
+        <v>D</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D11" t="e">
-        <f t="array" aca="1" ref="D11:E12" ca="1">_xll.xloObj($B$2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E11" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D11" t="str">
+        <f t="array" ref="D11:E12">_xll.xloVal($B$2)</f>
+        <v>X</v>
+      </c>
+      <c r="E11" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E12" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D12" t="str">
+        <v>C</v>
+      </c>
+      <c r="E12" t="str">
+        <v>D</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D14" t="e">
-        <f t="array" aca="1" ref="D14:E15" ca="1">_xll.xloObj($B$5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E14" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D14" t="str">
+        <f t="array" ref="D14:E15">_xll.xloVal($B$5)</f>
+        <v>X</v>
+      </c>
+      <c r="E14" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E15" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D15" t="str">
+        <v>C</v>
+      </c>
+      <c r="E15" t="str">
+        <v>D</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Expose ExcelArray object in python * Create custom converters in python * Change converter names in pyton * Change syntax for Array converter in python * Refactor of some converter code to support above * Harmonise ExcelRange and ExcelArray interfaces * Tidy messy numpy array code and fix numpy array of string creation. * Allow "register" of python workbook-attached module even if compile fails.
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BD8955-D969-452A-9336-986807517A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A56F6D-E8F4-4D0A-8962-58E5827BBB7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7668" yWindow="1476" windowWidth="14868" windowHeight="11604" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>pySum</t>
   </si>
@@ -143,6 +144,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>pyTestCustomConv</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>pyTestDFrame</t>
   </si>
 </sst>
 </file>
@@ -604,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,10 +738,6 @@
         <f>_xll.pyRoundTrip(C9)</f>
         <v>3.3</v>
       </c>
-      <c r="H9" t="e">
-        <f>xlo</f>
-        <v>#NAME?</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1039,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>{90160000-000F-0000-1000-0000000FF1CE}</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1058,11 +1064,11 @@
       </c>
       <c r="C36" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename")),100)&amp;"!"&amp;ADDRESS(ROW(F37),COLUMN(F37),4)</f>
-        <v>[PythonTest.xlsx]Sheet2!F37</v>
+        <v>[PythonTest.xlsx]Sheet1!F37</v>
       </c>
       <c r="D36" t="str">
         <f t="array" aca="1" ref="D36" ca="1">_xll.pyTestRange(E36:F37)</f>
-        <v>[PythonTest.xlsx]Sheet2!F37</v>
+        <v>[PythonTest.xlsx]Sheet1!F37</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1071,12 +1077,85 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>3</v>
       </c>
       <c r="F37">
         <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="b">
+        <f>C39=D39</f>
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <f>_xll.pyTestCustomConv(1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" t="b">
+        <f>C40=D40</f>
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f>2*SUM(E40:F40)</f>
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <f t="array" ref="D40">SUM(_xll.pyTestCustomConv(E40:F40))</f>
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" t="b">
+        <f>C42=D42</f>
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <f>F43</f>
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <f>_xll.pyTestDFrame(E42:G43,"B")</f>
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1089,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECBB5EF-8BCA-472B-B4EA-42C7538449FE}">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix strings! * Fix handling of numpy fixed-width string arrays * Add functions to handle UTF32/16 conversion in Core (built in codecvt functions are slow) * Add test project to test these string functions * Tidy up some string handling by building on PString * Add documenation for custom converters * Add pandas Dataframe converter * Add to_cache function in python * Fix ExcelArray at(i) function * Fix many conversion warnings
</commit_message>
<xml_diff>
--- a/test/PythonTest.xlsx
+++ b/test/PythonTest.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A56F6D-E8F4-4D0A-8962-58E5827BBB7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2533129B-1DAB-4B1B-A228-990614346CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="-108" windowWidth="22188" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>pySum</t>
   </si>
@@ -153,6 +152,12 @@
   </si>
   <si>
     <t>pyTestDFrame</t>
+  </si>
+  <si>
+    <t>pyTestDFrame:index</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -192,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -314,11 +319,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,6 +357,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,16 +661,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1045,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1054,7 +1102,7 @@
         <v>{90160000-000F-0000-1000-0000000FF1CE}</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1062,30 +1110,30 @@
         <f ca="1">C36=D36</f>
         <v>1</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C36" s="21" t="str">
         <f ca="1">MID(CELL("filename"),FIND("[",CELL("filename")),100)&amp;"!"&amp;ADDRESS(ROW(F37),COLUMN(F37),4)</f>
         <v>[PythonTest.xlsx]Sheet1!F37</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D36" s="21" t="str">
         <f t="array" aca="1" ref="D36" ca="1">_xll.pyTestRange(E36:F37)</f>
         <v>[PythonTest.xlsx]Sheet1!F37</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E37" s="7">
         <v>3</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1101,7 +1149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" t="b">
         <f>C40=D40</f>
         <v>1</v>
@@ -1114,48 +1162,126 @@
         <f t="array" ref="D40">SUM(_xll.pyTestCustomConv(E40:F40))</f>
         <v>14</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="9">
         <v>3</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="b">
-        <f>C42=D42</f>
-        <v>1</v>
+      <c r="B42">
+        <v>2</v>
       </c>
       <c r="C42">
         <f>F43</f>
         <v>2</v>
       </c>
       <c r="D42">
-        <f>_xll.pyTestDFrame(E42:G43,"B")</f>
+        <f>_xll.pyTestFrameFetch(H42,,"B")</f>
         <v>2</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
+      <c r="H42" t="str">
+        <f>_xll.pyTestDFrame(E42:G43)</f>
+        <v>欣[PythonTest.xlsx]Sheet1!R42C8_x0000__x0000__x0000__x0000_</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+      <c r="F43" s="19">
         <v>2</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="20">
         <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="b">
+        <f>C45=D45</f>
+        <v>1</v>
+      </c>
+      <c r="C45" t="str">
+        <f>G46</f>
+        <v>Foo</v>
+      </c>
+      <c r="D45" t="str">
+        <f>_xll.pyTestFrameFetch(H45,0,"B")</f>
+        <v>Foo</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" t="str">
+        <f>_xll.pyTestDFrameIndex(E45:G47)</f>
+        <v>欣[PythonTest.xlsx]Sheet1!R45C4_x0000__x0000__x0000__x0000_</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B46" t="b">
+        <f t="shared" ref="B46:B47" si="0">C46=D46</f>
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <f>F47</f>
+        <v>2.1</v>
+      </c>
+      <c r="D46">
+        <f t="array" ref="D46:D47">TRANSPOSE(_xll.pyTestFrameFetch(H45,1))</f>
+        <v>2.1</v>
+      </c>
+      <c r="E46" s="22">
+        <v>0</v>
+      </c>
+      <c r="F46" s="23">
+        <v>5.3</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B47" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C47" t="str">
+        <f>G47</f>
+        <v>Bar</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Bar</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1</v>
+      </c>
+      <c r="F47" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>